<commit_message>
scrape time randomized to mimic human behavior
</commit_message>
<xml_diff>
--- a/database_text.xlsx
+++ b/database_text.xlsx
@@ -7,9 +7,9 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="technicals" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="puts" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="calls" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="technicalsRDFN" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="putsRDFN" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="callsRDFN" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -538,7 +538,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:46</t>
+          <t>2020-02-20 22:04:50</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -887,7 +887,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1879,7 +1879,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:48</t>
+          <t>2020-02-20 22:04:51</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2208,7 +2208,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2332,7 +2332,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2394,7 +2394,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2580,7 +2580,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -2890,7 +2890,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -2952,7 +2952,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -3014,7 +3014,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -3076,7 +3076,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -3262,7 +3262,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -3510,7 +3510,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -3634,7 +3634,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -3696,7 +3696,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -3758,7 +3758,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2020-02-20 21:57:50</t>
+          <t>2020-02-20 22:04:53</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">

</xml_diff>

<commit_message>
testing mode added to avoid bot detection
</commit_message>
<xml_diff>
--- a/database_text.xlsx
+++ b/database_text.xlsx
@@ -372,7 +372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -845,6 +845,123 @@
       <c r="W4" t="inlineStr">
         <is>
           <t>1,851,284</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>29.25</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1,149,019</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>32.77</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>14.70</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>32.53</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>32.43</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>32.43</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:48</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>32.77</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>31.97</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Feb 11, 2020</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>-0.94</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>3.038B</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>32.66</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>+0.68%</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>32.21</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>+0.22</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>1,921,495</t>
         </is>
       </c>
     </row>
@@ -28197,7 +28314,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32542,6 +32659,1122 @@
       <c r="L70" t="inlineStr">
         <is>
           <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>115.63%</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>18.00</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>101.17%</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>19.00</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>105.47%</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>50.00%</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>21.00</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>25.00%</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>22.00</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>25.00%</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>23.00</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>57.42%</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>24.00</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>69.73%</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>25.00</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>55.47%</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>26.00</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>+0.05</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>51.56%</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>+33.33%</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>27.00</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>+0.10</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>52.15%</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>+40.00%</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>28.00</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>464</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>+0.05</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>47.75%</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>+14.29%</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>29.00</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>-0.07</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>45.75%</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>0.58</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>-10.77%</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>0.95</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>44.63%</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>0.95</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>31.00</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>1.30</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>+0.06</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>42.33%</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>+4.72%</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>32.00</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>4.60</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>49.71%</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>5.75</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>37.00</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>6.00</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>5.50</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>55.86%</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>6.65</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>38.00</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>7.40</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>-1.10</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:50</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>66.99%</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>7.90</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>-12.22%</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -32556,7 +33789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37459,6 +38692,1370 @@
       <c r="L79" t="inlineStr">
         <is>
           <t>50</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>16.60</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>14.20</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>200.39%</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>14.10</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>18.00</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>14.30</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>11.90</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>152.73%</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>11.09</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>13.00</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>11.00</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>133.98%</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>11.22</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>21.00</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>12.00</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>10.30</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>132.32%</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>6.60</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>22.00</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>10.30</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8.80</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>75.59%</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>8.70</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>23.00</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>8.70</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>8.30</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>+0.32</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>60.94%</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>8.32</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>+4.00%</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>24.00</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>7.80</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>7.40</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>+1.65</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>65.04%</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>7.60</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>+27.73%</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>25.00</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>6.90</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>6.40</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>+0.41</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>61.04%</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>6.41</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>+6.83%</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>26.00</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>5.90</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>5.40</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>+0.42</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>52.93%</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>5.60</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>+8.11%</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>27.00</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>4.80</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>4.60</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>+0.33</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>53.13%</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>4.78</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>+7.42%</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>28.00</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>465</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>3.70</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>+0.15</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>52.69%</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>3.70</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>+4.23%</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>29.00</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>3.10</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2.95</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>+0.26</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>46.44%</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>3.10</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>+9.15%</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>621</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2.45</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2.30</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>+0.28</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>46.73%</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>2.36</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>+13.46%</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>31.00</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>514</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>1.65</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>+0.20</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>44.29%</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>+12.90%</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>32.00</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>1.15</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>-0.10</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>41.99%</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>-9.09%</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>33.00</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>214</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>0.90</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>+0.10</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>42.58%</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>+13.33%</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>34.00</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>+0.10</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>41.90%</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>+20.00%</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>35.00</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>+0.02</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>43.95%</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>+5.71%</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>36.00</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>44.04%</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>37.00</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>+0.09</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>12.50%</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>+56.25%</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>38.00</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>-0.03</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>12.50%</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>-20.00%</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>39.00</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>+0.03</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2020-02-22 11:23:52</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>25.00%</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>+42.86%</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>RDFN</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>234</t>
         </is>
       </c>
     </row>

</xml_diff>